<commit_message>
function to instantiate Creator objs in csv2json
</commit_message>
<xml_diff>
--- a/figleaf/test_spreadsheet.xlsx
+++ b/figleaf/test_spreadsheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scarlettv/basic_figshare/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scarlettv/figleaf/figleaf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFF585F-002F-6D41-8AF0-78BB504E190D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9166DBAB-0124-3545-AB35-9CD228B8660F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="2600" windowWidth="28040" windowHeight="17440" xr2:uid="{F994D32C-DC09-7D4F-B37C-ED4B2EAE8784}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Virginia Scarlett</t>
   </si>
@@ -87,15 +87,63 @@
   </si>
   <si>
     <t>William Shakespeare</t>
+  </si>
+  <si>
+    <t>nameIdentifiers</t>
+  </si>
+  <si>
+    <t>nameIdentifierScheme</t>
+  </si>
+  <si>
+    <t>schemeURI</t>
+  </si>
+  <si>
+    <t>Affiliations</t>
+  </si>
+  <si>
+    <t>0000-0002-4156-2849</t>
+  </si>
+  <si>
+    <t>ORCID</t>
+  </si>
+  <si>
+    <t>https://orcid.org</t>
+  </si>
+  <si>
+    <t>University of California, Berkeley</t>
+  </si>
+  <si>
+    <t>HHMI Janelia Research Campus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF24292F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -122,8 +170,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,119 +489,191 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F50D26F-5E03-AC45-84A4-9E66DD8565A6}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D9" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D11" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="C12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C8">
+      <c r="C13" s="3">
         <v>2023</v>
       </c>
+      <c r="D13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
clean up code for create_creators w **kwargs
</commit_message>
<xml_diff>
--- a/figleaf/test_spreadsheet.xlsx
+++ b/figleaf/test_spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scarlettv/figleaf/figleaf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75BBE5F-33AE-5D48-A68A-C9D887092E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C03CA1-04DB-7D4B-8955-F169A088EDB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="2600" windowWidth="28040" windowHeight="17440" xr2:uid="{F994D32C-DC09-7D4F-B37C-ED4B2EAE8784}"/>
   </bookViews>
@@ -95,9 +95,6 @@
     <t>schemeURI</t>
   </si>
   <si>
-    <t>Affiliations</t>
-  </si>
-  <si>
     <t>0000-0002-4156-2849</t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t>types</t>
+  </si>
+  <si>
+    <t>affiliations</t>
   </si>
 </sst>
 </file>
@@ -510,7 +510,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -568,7 +568,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -582,7 +582,7 @@
         <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -596,7 +596,7 @@
         <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -607,10 +607,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -621,10 +621,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -671,16 +671,16 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -709,27 +709,27 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>